<commit_message>
Cut the log according to results given by the classifier on ngrams
</commit_message>
<xml_diff>
--- a/results/february.xlsx
+++ b/results/february.xlsx
@@ -189,7 +189,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,12 +325,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
@@ -652,7 +646,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="52">
+  <cellStyleXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -695,27 +689,30 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="52">
+  <cellStyles count="60">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -749,6 +746,10 @@
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -759,6 +760,10 @@
     <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -769,18 +774,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1056,20 +1050,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R42"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="125" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:XFD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B1"/>
+      <c r="C1"/>
+      <c r="D1"/>
+      <c r="E1"/>
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1100,25 +1104,19 @@
       <c r="K2" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="b">
-        <v>1</v>
+      <c r="C3" t="b">
+        <v>0</v>
       </c>
       <c r="D3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -1127,13 +1125,13 @@
         <v>0</v>
       </c>
       <c r="G3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" t="b">
         <v>1</v>
       </c>
       <c r="I3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" t="b">
         <v>0</v>
@@ -1142,21 +1140,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="b">
         <v>0</v>
       </c>
-      <c r="C4" s="1" t="b">
+      <c r="C4" t="b">
         <v>0</v>
       </c>
       <c r="D4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -1171,20 +1169,20 @@
         <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
-      <c r="C5" s="1" t="b">
+      <c r="C5" t="b">
         <v>0</v>
       </c>
       <c r="D5" t="b">
@@ -1203,7 +1201,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="b">
         <v>0</v>
@@ -1212,49 +1210,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="b">
+      <c r="C6" t="b">
         <v>1</v>
       </c>
       <c r="D6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
       </c>
       <c r="H6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="b">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="b">
         <v>0</v>
       </c>
       <c r="D7" t="b">
@@ -1264,7 +1262,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
@@ -1279,24 +1277,24 @@
         <v>0</v>
       </c>
       <c r="K7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
       </c>
-      <c r="C8" s="1" t="b">
-        <v>0</v>
+      <c r="C8" t="b">
+        <v>1</v>
       </c>
       <c r="D8" t="b">
         <v>1</v>
       </c>
       <c r="E8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -1305,30 +1303,30 @@
         <v>0</v>
       </c>
       <c r="H8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
       </c>
       <c r="J8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
       </c>
-      <c r="C9" s="1" t="b">
-        <v>0</v>
+      <c r="C9" t="b">
+        <v>1</v>
       </c>
       <c r="D9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -1346,20 +1344,20 @@
         <v>0</v>
       </c>
       <c r="J9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" t="b">
         <v>1</v>
       </c>
       <c r="D10" t="b">
@@ -1375,7 +1373,7 @@
         <v>1</v>
       </c>
       <c r="H10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
@@ -1387,33 +1385,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
       </c>
-      <c r="C11" s="1" t="b">
-        <v>0</v>
+      <c r="C11" t="b">
+        <v>1</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
       </c>
       <c r="E11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" t="b">
         <v>0</v>
       </c>
       <c r="H11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="b">
         <v>1</v>
@@ -1422,15 +1420,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
       </c>
-      <c r="C12" s="1" t="b">
-        <v>0</v>
+      <c r="C12" t="b">
+        <v>1</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -1445,10 +1443,10 @@
         <v>1</v>
       </c>
       <c r="H12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="b">
         <v>0</v>
@@ -1457,15 +1455,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13" t="b">
         <v>0</v>
       </c>
-      <c r="C13" s="1" t="b">
-        <v>0</v>
+      <c r="C13" t="b">
+        <v>1</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -1474,36 +1472,36 @@
         <v>1</v>
       </c>
       <c r="F13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="b">
         <v>0</v>
       </c>
       <c r="H13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
       <c r="B14" t="b">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C14" t="b">
+        <v>1</v>
       </c>
       <c r="D14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="b">
         <v>1</v>
@@ -1527,18 +1525,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
       <c r="B15" t="b">
         <v>0</v>
       </c>
-      <c r="C15" s="1" t="b">
-        <v>1</v>
+      <c r="C15" t="b">
+        <v>0</v>
       </c>
       <c r="D15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -1553,7 +1551,7 @@
         <v>1</v>
       </c>
       <c r="I15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="b">
         <v>1</v>
@@ -1562,15 +1560,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
       <c r="B16" t="b">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C16" t="b">
+        <v>0</v>
       </c>
       <c r="D16" t="b">
         <v>1</v>
@@ -1602,28 +1600,28 @@
         <v>24</v>
       </c>
       <c r="B17" t="b">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C17" t="b">
         <v>1</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>
       </c>
       <c r="E17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" t="b">
         <v>1</v>
       </c>
       <c r="G17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" t="b">
         <v>1</v>
       </c>
       <c r="I17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" t="b">
         <v>1</v>
@@ -1637,10 +1635,10 @@
         <v>25</v>
       </c>
       <c r="B18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C18" t="b">
+        <v>1</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
@@ -1655,13 +1653,13 @@
         <v>0</v>
       </c>
       <c r="H18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" t="b">
         <v>0</v>
       </c>
       <c r="J18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18" t="b">
         <v>1</v>
@@ -1674,26 +1672,26 @@
       <c r="B19" t="b">
         <v>1</v>
       </c>
-      <c r="C19" s="1" t="b">
-        <v>1</v>
+      <c r="C19" t="b">
+        <v>0</v>
       </c>
       <c r="D19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" t="b">
         <v>1</v>
       </c>
       <c r="G19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" t="b">
         <v>1</v>
       </c>
       <c r="I19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="b">
         <v>1</v>
@@ -1709,7 +1707,7 @@
       <c r="B20" t="b">
         <v>1</v>
       </c>
-      <c r="C20" s="1" t="b">
+      <c r="C20" t="b">
         <v>0</v>
       </c>
       <c r="D20" t="b">
@@ -1725,13 +1723,13 @@
         <v>0</v>
       </c>
       <c r="H20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" t="b">
         <v>1</v>
       </c>
       <c r="J20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20" t="b">
         <v>1</v>
@@ -1742,9 +1740,9 @@
         <v>28</v>
       </c>
       <c r="B21" t="b">
-        <v>0</v>
-      </c>
-      <c r="C21" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C21" t="b">
         <v>0</v>
       </c>
       <c r="D21" t="b">
@@ -1777,13 +1775,13 @@
         <v>29</v>
       </c>
       <c r="B22" t="b">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C22" t="b">
         <v>1</v>
       </c>
       <c r="D22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" t="b">
         <v>1</v>
@@ -1798,7 +1796,7 @@
         <v>1</v>
       </c>
       <c r="I22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="b">
         <v>0</v>
@@ -1815,51 +1813,51 @@
         <v>1</v>
       </c>
       <c r="C23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" t="b">
         <v>1</v>
       </c>
       <c r="G23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" t="b">
         <v>1</v>
       </c>
       <c r="I23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
       </c>
-      <c r="C24" s="4" t="b">
-        <v>0</v>
+      <c r="C24" t="b">
+        <v>1</v>
       </c>
       <c r="D24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" t="b">
         <v>1</v>
       </c>
       <c r="F24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" t="b">
         <v>0</v>
@@ -1885,7 +1883,7 @@
         <v>1</v>
       </c>
       <c r="C25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" t="b">
         <v>0</v>
@@ -1917,10 +1915,10 @@
         <v>34</v>
       </c>
       <c r="B26" t="b">
-        <v>0</v>
-      </c>
-      <c r="C26" s="2" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="C26" t="b">
+        <v>0</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
@@ -1929,7 +1927,7 @@
         <v>0</v>
       </c>
       <c r="F26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26" t="b">
         <v>1</v>
@@ -1954,14 +1952,14 @@
       <c r="B27" t="b">
         <v>0</v>
       </c>
-      <c r="C27" s="2" t="b">
-        <v>0</v>
+      <c r="C27" t="b">
+        <v>1</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
       </c>
       <c r="E27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27" t="b">
         <v>1</v>
@@ -1979,7 +1977,7 @@
         <v>1</v>
       </c>
       <c r="K27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -1987,16 +1985,16 @@
         <v>36</v>
       </c>
       <c r="B28" t="b">
-        <v>1</v>
-      </c>
-      <c r="C28" s="2" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="C28" t="b">
+        <v>1</v>
       </c>
       <c r="D28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28" t="b">
         <v>1</v>
@@ -2005,7 +2003,7 @@
         <v>0</v>
       </c>
       <c r="H28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" t="b">
         <v>0</v>
@@ -2022,16 +2020,16 @@
         <v>37</v>
       </c>
       <c r="B29" t="b">
-        <v>0</v>
-      </c>
-      <c r="C29" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C29" t="b">
         <v>0</v>
       </c>
       <c r="D29" t="b">
         <v>0</v>
       </c>
       <c r="E29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" t="b">
         <v>0</v>
@@ -2040,7 +2038,7 @@
         <v>0</v>
       </c>
       <c r="H29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29" t="b">
         <v>1</v>
@@ -2057,10 +2055,10 @@
         <v>38</v>
       </c>
       <c r="B30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" t="b">
         <v>1</v>
@@ -2075,10 +2073,10 @@
         <v>1</v>
       </c>
       <c r="H30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" t="b">
         <v>0</v>
@@ -2095,7 +2093,7 @@
         <v>1</v>
       </c>
       <c r="C31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" t="b">
         <v>1</v>
@@ -2113,10 +2111,10 @@
         <v>1</v>
       </c>
       <c r="I31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K31" t="b">
         <v>0</v>
@@ -2127,13 +2125,13 @@
         <v>40</v>
       </c>
       <c r="B32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32" t="b">
         <v>1</v>
@@ -2154,7 +2152,7 @@
         <v>0</v>
       </c>
       <c r="K32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -2162,10 +2160,10 @@
         <v>41</v>
       </c>
       <c r="B33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" t="b">
         <v>1</v>
@@ -2174,22 +2172,22 @@
         <v>0</v>
       </c>
       <c r="F33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33" t="b">
         <v>1</v>
       </c>
       <c r="H33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33" t="b">
         <v>1</v>
       </c>
       <c r="J33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -2200,7 +2198,7 @@
         <v>0</v>
       </c>
       <c r="C34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" t="b">
         <v>1</v>
@@ -2209,7 +2207,7 @@
         <v>1</v>
       </c>
       <c r="F34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34" t="b">
         <v>0</v>
@@ -2218,13 +2216,13 @@
         <v>1</v>
       </c>
       <c r="I34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2241,10 +2239,10 @@
         <v>1</v>
       </c>
       <c r="E35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35" t="b">
         <v>0</v>
@@ -2253,13 +2251,13 @@
         <v>0</v>
       </c>
       <c r="I35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J35" t="b">
         <v>0</v>
       </c>
       <c r="K35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -2267,7 +2265,7 @@
         <v>44</v>
       </c>
       <c r="B36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36" t="b">
         <v>1</v>
@@ -2282,10 +2280,10 @@
         <v>1</v>
       </c>
       <c r="G36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36" t="b">
         <v>0</v>
@@ -2302,10 +2300,10 @@
         <v>45</v>
       </c>
       <c r="B37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" t="b">
         <v>0</v>
@@ -2320,10 +2318,10 @@
         <v>1</v>
       </c>
       <c r="H37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" t="b">
         <v>0</v>
@@ -2343,22 +2341,22 @@
         <v>1</v>
       </c>
       <c r="D38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38" t="b">
         <v>1</v>
       </c>
       <c r="H38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" t="b">
         <v>0</v>
@@ -2384,7 +2382,7 @@
         <v>0</v>
       </c>
       <c r="F39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G39" t="b">
         <v>0</v>
@@ -2410,7 +2408,7 @@
         <v>1</v>
       </c>
       <c r="C40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" t="b">
         <v>0</v>
@@ -2419,7 +2417,7 @@
         <v>0</v>
       </c>
       <c r="F40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40" t="b">
         <v>1</v>
@@ -2445,22 +2443,22 @@
         <v>1</v>
       </c>
       <c r="C41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41" t="b">
         <v>1</v>
       </c>
       <c r="H41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41" t="b">
         <v>0</v>
@@ -2489,13 +2487,13 @@
         <v>0</v>
       </c>
       <c r="F42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42" t="b">
         <v>1</v>
       </c>
       <c r="H42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Added the web interface
</commit_message>
<xml_diff>
--- a/results/february.xlsx
+++ b/results/february.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400"/>
+    <workbookView xWindow="400" yWindow="460" windowWidth="28800" windowHeight="16400"/>
   </bookViews>
   <sheets>
     <sheet name="february" sheetId="1" r:id="rId1"/>
@@ -1057,7 +1057,7 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>